<commit_message>
Fix tables and data up
</commit_message>
<xml_diff>
--- a/results/tables/MyMachine.xlsx
+++ b/results/tables/MyMachine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\RSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\napier-constant\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
   <si>
     <r>
       <rPr>
@@ -51,6 +51,12 @@
 Точност
 </t>
     </r>
+  </si>
+  <si>
+    <t>Ускорение</t>
+  </si>
+  <si>
+    <t>Ефективност</t>
   </si>
 </sst>
 </file>
@@ -123,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -135,6 +141,9 @@
       <alignment textRotation="135" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -417,15 +426,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="25" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -509,7 +518,7 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+      <c r="A2" s="7">
         <v>1000</v>
       </c>
       <c r="B2" s="1">
@@ -586,7 +595,7 @@
       </c>
     </row>
     <row r="3" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1">
         <v>2.6932441762599999</v>
       </c>
@@ -661,7 +670,7 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1">
         <v>2.6594245949899999</v>
       </c>
@@ -736,7 +745,7 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1">
         <v>2.6920208257799998</v>
       </c>
@@ -811,7 +820,7 @@
       </c>
     </row>
     <row r="6" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1">
         <v>2.6954575761099999</v>
       </c>
@@ -886,7 +895,7 @@
       </c>
     </row>
     <row r="7" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1">
         <v>2.6740049273499999</v>
       </c>
@@ -961,7 +970,7 @@
       </c>
     </row>
     <row r="8" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1">
         <v>2.7034174467400001</v>
       </c>
@@ -1036,7 +1045,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1">
         <v>2.6942239619600001</v>
       </c>
@@ -1111,7 +1120,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1">
         <v>2.6905227247500001</v>
       </c>
@@ -1186,7 +1195,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1">
         <v>2.70716960754</v>
       </c>
@@ -1261,7 +1270,7 @@
       </c>
     </row>
     <row r="12" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="2">
         <f>AVERAGE(B2:B11)</f>
         <v>2.683859984598</v>
@@ -1359,1713 +1368,2319 @@
         <v>0.83135322143039991</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+    <row r="13" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2">
+        <f>$B$12/B12</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" ref="C13:Y13" si="1">$B$12/C12</f>
+        <v>1.9777772619117602</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="1"/>
+        <v>2.8496695253745705</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.3606804846561289</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.6686782566399021</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>4.0500150979665648</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>4.4285350354507571</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>4.6865073366391572</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>4.2916883209880874</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="1"/>
+        <v>4.1363545325307136</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="1"/>
+        <v>4.0557748820042754</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.9462310812292101</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.800997572962507</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.6802580391495647</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.713667643775592</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.6797644460761005</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.5977639142459545</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.4908285287709919</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.4896842995476227</v>
+      </c>
+      <c r="U13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.4088338626108783</v>
+      </c>
+      <c r="V13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.4076848441342342</v>
+      </c>
+      <c r="W13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.3180308227508979</v>
+      </c>
+      <c r="X13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.2682227047802215</v>
+      </c>
+      <c r="Y13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.2283028626270744</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2">
+        <f>B13/B1</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" ref="C14:Y14" si="2">C13/C1</f>
+        <v>0.98888863095588009</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.94988984179152347</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.84017012116403222</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.73373565132798046</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.67500251632776076</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.632647862207251</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.58581341707989465</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.47685425788756525</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.41363545325307138</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.36870680745493412</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.32885259010243417</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.2923844286894236</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.26287557422496893</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.24757784291837279</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.22998527787975628</v>
+      </c>
+      <c r="R14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.21163317142623261</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.1939349182650551</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.18366759471303276</v>
+      </c>
+      <c r="U14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.17044169313054391</v>
+      </c>
+      <c r="V14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.16227070686353495</v>
+      </c>
+      <c r="W14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.15081958285231353</v>
+      </c>
+      <c r="X14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.14209663933827049</v>
+      </c>
+      <c r="Y14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.13451261927612809</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
         <v>2000</v>
       </c>
-      <c r="B13">
-        <v>21.7836055245</v>
-      </c>
-      <c r="C13">
+      <c r="B15">
+        <v>21.2836055245</v>
+      </c>
+      <c r="C15">
         <v>10.6445935922</v>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>7.3855133038899998</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>5.9251442933799998</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>5.1614025225700004</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>4.7851229686299996</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>4.1805430823499998</v>
       </c>
-      <c r="I13">
+      <c r="I15">
         <v>3.8781378702999998</v>
       </c>
-      <c r="J13">
+      <c r="J15">
         <v>4.0167301764100003</v>
       </c>
-      <c r="K13">
+      <c r="K15">
         <v>4.0819175061499999</v>
       </c>
-      <c r="L13">
+      <c r="L15">
         <v>4.0676596898700002</v>
       </c>
-      <c r="M13">
+      <c r="M15">
         <v>3.9897769901900002</v>
       </c>
-      <c r="N13">
+      <c r="N15">
         <v>4.0338160284600004</v>
       </c>
-      <c r="O13">
+      <c r="O15">
         <v>3.9607564640400001</v>
       </c>
-      <c r="P13">
+      <c r="P15">
         <v>4.0130044642999998</v>
       </c>
-      <c r="Q13">
+      <c r="Q15">
         <v>4.0794471198000002</v>
       </c>
-      <c r="R13">
+      <c r="R15">
         <v>4.0527671051</v>
       </c>
-      <c r="S13">
+      <c r="S15">
         <v>4.0323155588899997</v>
       </c>
-      <c r="T13">
+      <c r="T15">
         <v>4.0822033098799997</v>
       </c>
-      <c r="U13">
+      <c r="U15">
         <v>4.2644083172</v>
       </c>
-      <c r="V13">
+      <c r="V15">
         <v>4.4592932989699996</v>
       </c>
-      <c r="W13">
+      <c r="W15">
         <v>4.2812786321800003</v>
       </c>
-      <c r="X13">
+      <c r="X15">
         <v>4.1631532677700003</v>
       </c>
-      <c r="Y13">
+      <c r="Y15">
         <v>4.2646791201800003</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14">
-        <v>21.678442780200001</v>
-      </c>
-      <c r="C14">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16">
+        <v>21.264427802</v>
+      </c>
+      <c r="C16">
         <v>10.6528633467</v>
       </c>
-      <c r="D14">
+      <c r="D16">
         <v>7.2888816429099998</v>
       </c>
-      <c r="E14">
+      <c r="E16">
         <v>5.8867668532400002</v>
       </c>
-      <c r="F14">
+      <c r="F16">
         <v>5.0686343437400003</v>
       </c>
-      <c r="G14">
+      <c r="G16">
         <v>4.6047366046300002</v>
       </c>
-      <c r="H14">
+      <c r="H16">
         <v>4.1985025305899999</v>
       </c>
-      <c r="I14">
+      <c r="I16">
         <v>3.8417077641100001</v>
       </c>
-      <c r="J14">
+      <c r="J16">
         <v>4.0474611826000002</v>
       </c>
-      <c r="K14">
+      <c r="K16">
         <v>4.0146549413499999</v>
       </c>
-      <c r="L14">
+      <c r="L16">
         <v>3.9040540311199998</v>
       </c>
-      <c r="M14">
+      <c r="M16">
         <v>3.9139659727799998</v>
       </c>
-      <c r="N14">
+      <c r="N16">
         <v>3.99790029003</v>
       </c>
-      <c r="O14">
+      <c r="O16">
         <v>4.0482688544599998</v>
       </c>
-      <c r="P14">
+      <c r="P16">
         <v>3.9612131973400002</v>
       </c>
-      <c r="Q14">
+      <c r="Q16">
         <v>3.9909395481700001</v>
       </c>
-      <c r="R14">
+      <c r="R16">
         <v>4.1002049970599996</v>
       </c>
-      <c r="S14">
+      <c r="S16">
         <v>4.1707546994799998</v>
       </c>
-      <c r="T14">
+      <c r="T16">
         <v>4.1003589521099997</v>
       </c>
-      <c r="U14">
+      <c r="U16">
         <v>4.1283894288900003</v>
       </c>
-      <c r="V14">
+      <c r="V16">
         <v>4.1777486008800002</v>
       </c>
-      <c r="W14">
+      <c r="W16">
         <v>4.2506632896600003</v>
       </c>
-      <c r="X14">
+      <c r="X16">
         <v>4.4318127180299998</v>
       </c>
-      <c r="Y14">
+      <c r="Y16">
         <v>4.4240293035700002</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15">
-        <v>21.503612614400001</v>
-      </c>
-      <c r="C15">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17">
+        <v>21.343612614400001</v>
+      </c>
+      <c r="C17">
         <v>10.6090836635</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <v>7.3058692005800001</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <v>5.8378553351500004</v>
       </c>
-      <c r="F15">
+      <c r="F17">
         <v>5.2528928745299996</v>
       </c>
-      <c r="G15">
+      <c r="G17">
         <v>4.6702164489499998</v>
       </c>
-      <c r="H15">
+      <c r="H17">
         <v>4.2043563751399997</v>
       </c>
-      <c r="I15">
+      <c r="I17">
         <v>3.8983359828099999</v>
       </c>
-      <c r="J15">
+      <c r="J17">
         <v>4.03301506746</v>
       </c>
-      <c r="K15">
+      <c r="K17">
         <v>3.9579777728400001</v>
       </c>
-      <c r="L15">
+      <c r="L17">
         <v>3.9662905558100001</v>
       </c>
-      <c r="M15">
+      <c r="M17">
         <v>3.9815403952400001</v>
       </c>
-      <c r="N15">
+      <c r="N17">
         <v>4.0692383212300003</v>
       </c>
-      <c r="O15">
+      <c r="O17">
         <v>3.9945653868800002</v>
       </c>
-      <c r="P15">
+      <c r="P17">
         <v>4.0039708559199996</v>
       </c>
-      <c r="Q15">
+      <c r="Q17">
         <v>4.0115363647700004</v>
       </c>
-      <c r="R15">
+      <c r="R17">
         <v>4.3925245745800003</v>
       </c>
-      <c r="S15">
+      <c r="S17">
         <v>4.11063170124</v>
       </c>
-      <c r="T15">
+      <c r="T17">
         <v>4.2115527866500004</v>
       </c>
-      <c r="U15">
+      <c r="U17">
         <v>4.1446415551499998</v>
       </c>
-      <c r="V15">
+      <c r="V17">
         <v>4.1863290287800003</v>
       </c>
-      <c r="W15">
+      <c r="W17">
         <v>4.28044411688</v>
       </c>
-      <c r="X15">
+      <c r="X17">
         <v>4.2294557846999998</v>
       </c>
-      <c r="Y15">
+      <c r="Y17">
         <v>4.0967433770700001</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16">
-        <v>21.6421512336</v>
-      </c>
-      <c r="C16">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18">
+        <v>20.151233600000001</v>
+      </c>
+      <c r="C18">
         <v>10.5750457819</v>
       </c>
-      <c r="D16">
+      <c r="D18">
         <v>7.3109284002499999</v>
       </c>
-      <c r="E16">
+      <c r="E18">
         <v>5.7523569925400002</v>
       </c>
-      <c r="F16">
+      <c r="F18">
         <v>5.0835281127799998</v>
       </c>
-      <c r="G16">
+      <c r="G18">
         <v>4.6797004745399997</v>
       </c>
-      <c r="H16">
+      <c r="H18">
         <v>4.1412209898399999</v>
       </c>
-      <c r="I16">
+      <c r="I18">
         <v>3.8353624476800001</v>
       </c>
-      <c r="J16">
+      <c r="J18">
         <v>4.02661724841</v>
       </c>
-      <c r="K16">
+      <c r="K18">
         <v>3.9839199875900002</v>
       </c>
-      <c r="L16">
+      <c r="L18">
         <v>3.9390041950799999</v>
       </c>
-      <c r="M16">
+      <c r="M18">
         <v>3.9017131249000001</v>
       </c>
-      <c r="N16">
+      <c r="N18">
         <v>3.96368003089</v>
       </c>
-      <c r="O16">
+      <c r="O18">
         <v>3.9823918850700002</v>
       </c>
-      <c r="P16">
+      <c r="P18">
         <v>4.0145187503399997</v>
       </c>
-      <c r="Q16">
+      <c r="Q18">
         <v>4.0765393432100003</v>
       </c>
-      <c r="R16">
+      <c r="R18">
         <v>4.0585206814900001</v>
       </c>
-      <c r="S16">
+      <c r="S18">
         <v>4.1014615070899998</v>
       </c>
-      <c r="T16">
+      <c r="T18">
         <v>4.1234352344699996</v>
       </c>
-      <c r="U16">
+      <c r="U18">
         <v>4.1240565812399996</v>
       </c>
-      <c r="V16">
+      <c r="V18">
         <v>4.2233895611400003</v>
       </c>
-      <c r="W16">
+      <c r="W18">
         <v>4.3107037837800002</v>
       </c>
-      <c r="X16">
+      <c r="X18">
         <v>4.1774071364900003</v>
       </c>
-      <c r="Y16">
+      <c r="Y18">
         <v>4.3923437760899997</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17">
-        <v>21.665028163900001</v>
-      </c>
-      <c r="C17">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19">
+        <v>21.102816390000001</v>
+      </c>
+      <c r="C19">
         <v>10.549764784300001</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>7.2511405502999997</v>
       </c>
-      <c r="E17">
+      <c r="E19">
         <v>5.80386245577</v>
       </c>
-      <c r="F17">
+      <c r="F19">
         <v>5.2216925028199999</v>
       </c>
-      <c r="G17">
+      <c r="G19">
         <v>4.6363522601999998</v>
       </c>
-      <c r="H17">
+      <c r="H19">
         <v>4.1624659966599999</v>
       </c>
-      <c r="I17">
+      <c r="I19">
         <v>3.84088706529</v>
       </c>
-      <c r="J17">
+      <c r="J19">
         <v>4.0324114847299999</v>
       </c>
-      <c r="K17">
+      <c r="K19">
         <v>3.9981324068699999</v>
       </c>
-      <c r="L17">
+      <c r="L19">
         <v>3.9394767186399999</v>
       </c>
-      <c r="M17">
+      <c r="M19">
         <v>3.9213806846399999</v>
       </c>
-      <c r="N17">
+      <c r="N19">
         <v>4.0115347857500003</v>
       </c>
-      <c r="O17">
+      <c r="O19">
         <v>4.0389703644399999</v>
       </c>
-      <c r="P17">
+      <c r="P19">
         <v>4.0317964540600002</v>
       </c>
-      <c r="Q17">
+      <c r="Q19">
         <v>4.0250974357800002</v>
       </c>
-      <c r="R17">
+      <c r="R19">
         <v>4.0272922820800003</v>
       </c>
-      <c r="S17">
+      <c r="S19">
         <v>4.0870055230400002</v>
       </c>
-      <c r="T17">
+      <c r="T19">
         <v>4.0866324781200003</v>
       </c>
-      <c r="U17">
+      <c r="U19">
         <v>4.17548388268</v>
       </c>
-      <c r="V17">
+      <c r="V19">
         <v>4.1570917812900001</v>
       </c>
-      <c r="W17">
+      <c r="W19">
         <v>4.2879200160100002</v>
       </c>
-      <c r="X17">
+      <c r="X19">
         <v>4.3498620523299998</v>
       </c>
-      <c r="Y17">
+      <c r="Y19">
         <v>4.5699786870999999</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18">
-        <v>21.655227543599999</v>
-      </c>
-      <c r="C18">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20">
+        <v>21.3452275436</v>
+      </c>
+      <c r="C20">
         <v>10.621024653699999</v>
       </c>
-      <c r="D18">
+      <c r="D20">
         <v>7.3024817948200003</v>
       </c>
-      <c r="E18">
+      <c r="E20">
         <v>5.8221653421899999</v>
       </c>
-      <c r="F18">
+      <c r="F20">
         <v>5.1149302050700003</v>
       </c>
-      <c r="G18">
+      <c r="G20">
         <v>4.62480760554</v>
       </c>
-      <c r="H18">
+      <c r="H20">
         <v>4.1946094417099999</v>
       </c>
-      <c r="I18">
+      <c r="I20">
         <v>3.8749640278099999</v>
       </c>
-      <c r="J18">
+      <c r="J20">
         <v>4.0231726029499999</v>
       </c>
-      <c r="K18">
+      <c r="K20">
         <v>4.0897127633099997</v>
       </c>
-      <c r="L18">
+      <c r="L20">
         <v>3.9469881458599998</v>
       </c>
-      <c r="M18">
+      <c r="M20">
         <v>3.9632426406499999</v>
       </c>
-      <c r="N18">
+      <c r="N20">
         <v>4.0093233596799998</v>
       </c>
-      <c r="O18">
+      <c r="O20">
         <v>3.9556266029599998</v>
       </c>
-      <c r="P18">
+      <c r="P20">
         <v>3.98301717941</v>
       </c>
-      <c r="Q18">
+      <c r="Q20">
         <v>4.0881218945000004</v>
       </c>
-      <c r="R18">
+      <c r="R20">
         <v>4.1366090493199996</v>
       </c>
-      <c r="S18">
+      <c r="S20">
         <v>4.1326377986500002</v>
       </c>
-      <c r="T18">
+      <c r="T20">
         <v>4.1149688912100002</v>
       </c>
-      <c r="U18">
+      <c r="U20">
         <v>4.0888825903299999</v>
       </c>
-      <c r="V18">
+      <c r="V20">
         <v>4.3363894067900004</v>
       </c>
-      <c r="W18">
+      <c r="W20">
         <v>4.1984452908899996</v>
       </c>
-      <c r="X18">
+      <c r="X20">
         <v>4.1119695311099997</v>
       </c>
-      <c r="Y18">
+      <c r="Y20">
         <v>4.4347449695199996</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19">
-        <v>21.709609202900001</v>
-      </c>
-      <c r="C19">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21">
+        <v>21.16092029</v>
+      </c>
+      <c r="C21">
         <v>10.5669903802</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>7.4104674430499999</v>
       </c>
-      <c r="E19">
+      <c r="E21">
         <v>5.7565232529400001</v>
       </c>
-      <c r="F19">
+      <c r="F21">
         <v>5.1909034674200001</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <v>4.5408196014</v>
       </c>
-      <c r="H19">
+      <c r="H21">
         <v>4.1908770187400002</v>
       </c>
-      <c r="I19">
+      <c r="I21">
         <v>3.8277503575499998</v>
       </c>
-      <c r="J19">
+      <c r="J21">
         <v>4.0076902519199997</v>
       </c>
-      <c r="K19">
+      <c r="K21">
         <v>3.9541367918199999</v>
       </c>
-      <c r="L19">
+      <c r="L21">
         <v>3.9768254232700002</v>
       </c>
-      <c r="M19">
+      <c r="M21">
         <v>3.9282522115199998</v>
       </c>
-      <c r="N19">
+      <c r="N21">
         <v>3.9926295008700001</v>
       </c>
-      <c r="O19">
+      <c r="O21">
         <v>3.9786859107799999</v>
       </c>
-      <c r="P19">
+      <c r="P21">
         <v>4.0073847103700002</v>
       </c>
-      <c r="Q19">
+      <c r="Q21">
         <v>4.0202723267399998</v>
       </c>
-      <c r="R19">
+      <c r="R21">
         <v>4.0905559632499999</v>
       </c>
-      <c r="S19">
+      <c r="S21">
         <v>4.1177977164900001</v>
       </c>
-      <c r="T19">
+      <c r="T21">
         <v>4.0855875575900003</v>
       </c>
-      <c r="U19">
+      <c r="U21">
         <v>4.0705508866800004</v>
       </c>
-      <c r="V19">
+      <c r="V21">
         <v>4.0525823590399996</v>
       </c>
-      <c r="W19">
+      <c r="W21">
         <v>4.2432730527000002</v>
       </c>
-      <c r="X19">
+      <c r="X21">
         <v>4.0928668679699998</v>
       </c>
-      <c r="Y19">
+      <c r="Y21">
         <v>4.0994593019799996</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20">
-        <v>21.875383654</v>
-      </c>
-      <c r="C20">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22">
+        <v>21.453836540000001</v>
+      </c>
+      <c r="C22">
         <v>10.5746676051</v>
       </c>
-      <c r="D20">
+      <c r="D22">
         <v>7.1724750484299999</v>
       </c>
-      <c r="E20">
+      <c r="E22">
         <v>5.8306557656000004</v>
       </c>
-      <c r="F20">
+      <c r="F22">
         <v>5.2731948080000004</v>
       </c>
-      <c r="G20">
+      <c r="G22">
         <v>4.6198814388200002</v>
       </c>
-      <c r="H20">
+      <c r="H22">
         <v>4.19441324771</v>
       </c>
-      <c r="I20">
+      <c r="I22">
         <v>3.8361930154100001</v>
       </c>
-      <c r="J20">
+      <c r="J22">
         <v>3.9897169872</v>
       </c>
-      <c r="K20">
+      <c r="K22">
         <v>3.9254518087200001</v>
       </c>
-      <c r="L20">
+      <c r="L22">
         <v>3.9893680224299999</v>
       </c>
-      <c r="M20">
+      <c r="M22">
         <v>3.9838655111899999</v>
       </c>
-      <c r="N20">
+      <c r="N22">
         <v>3.9647490315599998</v>
       </c>
-      <c r="O20">
+      <c r="O22">
         <v>4.0021699766300003</v>
       </c>
-      <c r="P20">
+      <c r="P22">
         <v>4.0054290865300004</v>
       </c>
-      <c r="Q20">
+      <c r="Q22">
         <v>4.0067696796999996</v>
       </c>
-      <c r="R20">
+      <c r="R22">
         <v>4.0963565156700001</v>
       </c>
-      <c r="S20">
+      <c r="S22">
         <v>4.1649395410599999</v>
       </c>
-      <c r="T20">
+      <c r="T22">
         <v>4.18099428906</v>
       </c>
-      <c r="U20">
+      <c r="U22">
         <v>4.1391868094499999</v>
       </c>
-      <c r="V20">
+      <c r="V22">
         <v>4.21920316816</v>
       </c>
-      <c r="W20">
+      <c r="W22">
         <v>4.2779958368999997</v>
       </c>
-      <c r="X20">
+      <c r="X22">
         <v>4.1861166497599998</v>
       </c>
-      <c r="Y20">
+      <c r="Y22">
         <v>4.3972695480499997</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21">
-        <v>21.582323907999999</v>
-      </c>
-      <c r="C21">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23">
+        <v>21.332323907999999</v>
+      </c>
+      <c r="C23">
         <v>10.6034954901</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>7.23401719638</v>
       </c>
-      <c r="E21">
+      <c r="E23">
         <v>5.7868772666400004</v>
       </c>
-      <c r="F21">
+      <c r="F23">
         <v>5.2049595631200001</v>
       </c>
-      <c r="G21">
+      <c r="G23">
         <v>4.6339825367599996</v>
       </c>
-      <c r="H21">
+      <c r="H23">
         <v>4.1717333009099997</v>
       </c>
-      <c r="I21">
+      <c r="I23">
         <v>3.8279532624099999</v>
       </c>
-      <c r="J21">
+      <c r="J23">
         <v>3.9682809182200001</v>
       </c>
-      <c r="K21">
+      <c r="K23">
         <v>4.0387224573399996</v>
       </c>
-      <c r="L21">
+      <c r="L23">
         <v>3.9399567425800002</v>
       </c>
-      <c r="M21">
+      <c r="M23">
         <v>3.9316684345200001</v>
       </c>
-      <c r="N21">
+      <c r="N23">
         <v>4.0013824373600002</v>
       </c>
-      <c r="O21">
+      <c r="O23">
         <v>3.9873701596400002</v>
       </c>
-      <c r="P21">
+      <c r="P23">
         <v>4.0204029911500001</v>
       </c>
-      <c r="Q21">
+      <c r="Q23">
         <v>4.0368911818099997</v>
       </c>
-      <c r="R21">
+      <c r="R23">
         <v>4.1027764410899996</v>
       </c>
-      <c r="S21">
+      <c r="S23">
         <v>4.1295054055999998</v>
       </c>
-      <c r="T21">
+      <c r="T23">
         <v>4.1940729675900004</v>
       </c>
-      <c r="U21">
+      <c r="U23">
         <v>4.1697713609699996</v>
       </c>
-      <c r="V21">
+      <c r="V23">
         <v>4.6445537218200004</v>
       </c>
-      <c r="W21">
+      <c r="W23">
         <v>4.3276309437</v>
       </c>
-      <c r="X21">
+      <c r="X23">
         <v>4.1645929448299999</v>
       </c>
-      <c r="Y21">
+      <c r="Y23">
         <v>4.5487964465599999</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22">
-        <v>21.645718648300001</v>
-      </c>
-      <c r="C22">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24">
+        <v>21.157186483</v>
+      </c>
+      <c r="C24">
         <v>10.6163929754</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>7.2697047655400002</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>5.8321013639999997</v>
       </c>
-      <c r="F22">
+      <c r="F24">
         <v>5.2379256807700001</v>
       </c>
-      <c r="G22">
+      <c r="G24">
         <v>4.6195182628199998</v>
       </c>
-      <c r="H22">
+      <c r="H24">
         <v>4.1442164023699997</v>
       </c>
-      <c r="I22">
+      <c r="I24">
         <v>3.8328987721900001</v>
       </c>
-      <c r="J22">
+      <c r="J24">
         <v>4.0224920426999997</v>
       </c>
-      <c r="K22">
+      <c r="K24">
         <v>3.9409724511299999</v>
       </c>
-      <c r="L22">
+      <c r="L24">
         <v>3.98203699895</v>
       </c>
-      <c r="M22">
+      <c r="M24">
         <v>4.0350070089000001</v>
       </c>
-      <c r="N22">
+      <c r="N24">
         <v>4.0486695323399999</v>
       </c>
-      <c r="O22">
+      <c r="O24">
         <v>4.0162264670800001</v>
       </c>
-      <c r="P22">
+      <c r="P24">
         <v>4.1254405976299999</v>
       </c>
-      <c r="Q22">
+      <c r="Q24">
         <v>4.0363910252900004</v>
       </c>
-      <c r="R22">
+      <c r="R24">
         <v>4.0906585999500003</v>
       </c>
-      <c r="S22">
+      <c r="S24">
         <v>4.1164034364299997</v>
       </c>
-      <c r="T22">
+      <c r="T24">
         <v>4.4035892053000003</v>
       </c>
-      <c r="U22">
+      <c r="U24">
         <v>4.1938238762199997</v>
       </c>
-      <c r="V22">
+      <c r="V24">
         <v>4.2721822575099999</v>
       </c>
-      <c r="W22">
+      <c r="W24">
         <v>4.1467732403999999</v>
       </c>
-      <c r="X22">
+      <c r="X24">
         <v>4.3939492508900004</v>
       </c>
-      <c r="Y22">
+      <c r="Y24">
         <v>4.2733886334599998</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="3">
-        <f>AVERAGE(B13:B22)</f>
-        <v>21.674110327339999</v>
-      </c>
-      <c r="C23" s="3">
-        <f t="shared" ref="C23:Y23" si="1">AVERAGE(C13:C22)</f>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="3">
+        <f>AVERAGE(B15:B24)</f>
+        <v>21.159519069550001</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" ref="C25:Y25" si="3">AVERAGE(C15:C24)</f>
         <v>10.601392227310001</v>
       </c>
-      <c r="D23" s="3">
-        <f t="shared" si="1"/>
+      <c r="D25" s="3">
+        <f t="shared" si="3"/>
         <v>7.2931479346149999</v>
       </c>
-      <c r="E23" s="3">
-        <f t="shared" si="1"/>
+      <c r="E25" s="3">
+        <f t="shared" si="3"/>
         <v>5.8234308921449998</v>
       </c>
-      <c r="F23" s="3">
-        <f t="shared" si="1"/>
+      <c r="F25" s="3">
+        <f t="shared" si="3"/>
         <v>5.1810064080819993</v>
       </c>
-      <c r="G23" s="3">
-        <f t="shared" si="1"/>
+      <c r="G25" s="3">
+        <f t="shared" si="3"/>
         <v>4.6415138202290001</v>
       </c>
-      <c r="H23" s="3">
-        <f t="shared" si="1"/>
+      <c r="H25" s="3">
+        <f t="shared" si="3"/>
         <v>4.1782938386020003</v>
       </c>
-      <c r="I23" s="3">
-        <f t="shared" si="1"/>
+      <c r="I25" s="3">
+        <f t="shared" si="3"/>
         <v>3.8494190565559996</v>
       </c>
-      <c r="J23" s="3">
-        <f t="shared" si="1"/>
+      <c r="J25" s="3">
+        <f t="shared" si="3"/>
         <v>4.0167587962600004</v>
       </c>
-      <c r="K23" s="3">
-        <f t="shared" si="1"/>
+      <c r="K25" s="3">
+        <f t="shared" si="3"/>
         <v>3.9985598887119997</v>
       </c>
-      <c r="L23" s="3">
-        <f t="shared" si="1"/>
+      <c r="L25" s="3">
+        <f t="shared" si="3"/>
         <v>3.9651660523609999</v>
       </c>
-      <c r="M23" s="3">
-        <f t="shared" si="1"/>
+      <c r="M25" s="3">
+        <f t="shared" si="3"/>
         <v>3.9550412974530005</v>
       </c>
-      <c r="N23" s="3">
-        <f t="shared" si="1"/>
+      <c r="N25" s="3">
+        <f t="shared" si="3"/>
         <v>4.009292331817</v>
       </c>
-      <c r="O23" s="3">
-        <f t="shared" si="1"/>
+      <c r="O25" s="3">
+        <f t="shared" si="3"/>
         <v>3.9965032071980007</v>
       </c>
-      <c r="P23" s="3">
-        <f t="shared" si="1"/>
+      <c r="P25" s="3">
+        <f t="shared" si="3"/>
         <v>4.0166178287049998</v>
       </c>
-      <c r="Q23" s="3">
-        <f t="shared" si="1"/>
+      <c r="Q25" s="3">
+        <f t="shared" si="3"/>
         <v>4.0372005919770002</v>
       </c>
-      <c r="R23" s="3">
-        <f t="shared" si="1"/>
+      <c r="R25" s="3">
+        <f t="shared" si="3"/>
         <v>4.1148266209590005</v>
       </c>
-      <c r="S23" s="3">
-        <f t="shared" si="1"/>
+      <c r="S25" s="3">
+        <f t="shared" si="3"/>
         <v>4.1163452887969996</v>
       </c>
-      <c r="T23" s="3">
-        <f t="shared" si="1"/>
+      <c r="T25" s="3">
+        <f t="shared" si="3"/>
         <v>4.1583395671980004</v>
       </c>
-      <c r="U23" s="3">
-        <f t="shared" si="1"/>
+      <c r="U25" s="3">
+        <f t="shared" si="3"/>
         <v>4.1499195288809991</v>
       </c>
-      <c r="V23" s="3">
-        <f t="shared" si="1"/>
+      <c r="V25" s="3">
+        <f t="shared" si="3"/>
         <v>4.2728763184379996</v>
       </c>
-      <c r="W23" s="3">
-        <f t="shared" si="1"/>
+      <c r="W25" s="3">
+        <f t="shared" si="3"/>
         <v>4.2605128203100007</v>
       </c>
-      <c r="X23" s="3">
-        <f t="shared" si="1"/>
+      <c r="X25" s="3">
+        <f t="shared" si="3"/>
         <v>4.2301186203879997</v>
       </c>
-      <c r="Y23" s="3">
-        <f t="shared" si="1"/>
+      <c r="Y25" s="3">
+        <f t="shared" si="3"/>
         <v>4.3501433163579994</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="2">
+        <f>$B$25/B25</f>
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" ref="C26:Y26" si="4">$B$25/C25</f>
+        <v>1.995918895920241</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="4"/>
+        <v>2.9012875179895823</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="4"/>
+        <v>3.6335142395338211</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="4"/>
+        <v>4.0840557611630564</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="4"/>
+        <v>4.5587538654589306</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.0641529501978937</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.4968084167175633</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.2678092319737013</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.2917849572001341</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.3363513129420834</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.3500121688176758</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.2776194196746351</v>
+      </c>
+      <c r="O26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.2945082169432833</v>
+      </c>
+      <c r="P26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.2679941114467574</v>
+      </c>
+      <c r="Q26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.241136422995587</v>
+      </c>
+      <c r="R26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.1422626075600162</v>
+      </c>
+      <c r="S26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.1403654419218707</v>
+      </c>
+      <c r="T26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.0884538714590466</v>
+      </c>
+      <c r="U26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.0987781623937991</v>
+      </c>
+      <c r="V26" s="2">
+        <f t="shared" si="4"/>
+        <v>4.9520551246110287</v>
+      </c>
+      <c r="W26" s="2">
+        <f t="shared" si="4"/>
+        <v>4.966425395713375</v>
+      </c>
+      <c r="X26" s="2">
+        <f t="shared" si="4"/>
+        <v>5.0021100986546765</v>
+      </c>
+      <c r="Y26" s="2">
+        <f t="shared" si="4"/>
+        <v>4.8640970034212678</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2">
+        <f>B26/B1</f>
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" ref="C27:Y27" si="5">C26/C1</f>
+        <v>0.99795944796012048</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.96709583932986076</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.90837855988345528</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.81681115223261125</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.7597923109098218</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.72345042145684191</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.68710105208969541</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.58531213688596684</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.52917849572001341</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.4851228466310985</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.44583434740147299</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.40597072459035655</v>
+      </c>
+      <c r="O27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.37817915835309168</v>
+      </c>
+      <c r="P27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.35119960742978384</v>
+      </c>
+      <c r="Q27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.32757102643722419</v>
+      </c>
+      <c r="R27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.30248603573882449</v>
+      </c>
+      <c r="S27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.28557585788454837</v>
+      </c>
+      <c r="T27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.26781336165573927</v>
+      </c>
+      <c r="U27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.25493890811968994</v>
+      </c>
+      <c r="V27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.23581214879100137</v>
+      </c>
+      <c r="W27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.22574660889606249</v>
+      </c>
+      <c r="X27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.21748304776759464</v>
+      </c>
+      <c r="Y27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.20267070847588617</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
         <v>3000</v>
       </c>
-      <c r="B24">
-        <v>76.599558188499998</v>
-      </c>
-      <c r="C24">
+      <c r="B28">
+        <v>72.599558188499998</v>
+      </c>
+      <c r="C28">
         <v>37.243651229400001</v>
       </c>
-      <c r="D24">
+      <c r="D28">
         <v>25.187038406300001</v>
       </c>
-      <c r="E24">
+      <c r="E28">
         <v>25.187038406300001</v>
       </c>
-      <c r="F24">
+      <c r="F28">
         <v>18.149819971300001</v>
       </c>
-      <c r="G24">
+      <c r="G28">
         <v>16.103472002099998</v>
       </c>
-      <c r="H24">
+      <c r="H28">
         <v>14.1915220509</v>
       </c>
-      <c r="I24">
+      <c r="I28">
         <v>13.2298773847</v>
       </c>
-      <c r="J24">
+      <c r="J28">
         <v>13.992014865</v>
       </c>
-      <c r="K24">
+      <c r="K28">
         <v>13.6787652963</v>
       </c>
-      <c r="L24">
+      <c r="L28">
         <v>13.438496735599999</v>
       </c>
-      <c r="M24">
+      <c r="M28">
         <v>13.215714309999999</v>
       </c>
-      <c r="N24">
+      <c r="N28">
         <v>13.432848953900001</v>
       </c>
-      <c r="O24">
+      <c r="O28">
         <v>13.347032437499999</v>
       </c>
-      <c r="P24">
+      <c r="P28">
         <v>13.320911003300001</v>
       </c>
-      <c r="Q24">
+      <c r="Q28">
         <v>13.2885228092</v>
       </c>
-      <c r="R24">
+      <c r="R28">
         <v>13.4341705988</v>
       </c>
-      <c r="S24">
+      <c r="S28">
         <v>13.3140347394</v>
       </c>
-      <c r="T24">
+      <c r="T28">
         <v>13.3140347394</v>
       </c>
-      <c r="U24">
+      <c r="U28">
         <v>13.3607091722</v>
       </c>
-      <c r="V24">
+      <c r="V28">
         <v>13.378952055599999</v>
       </c>
-      <c r="W24">
+      <c r="W28">
         <v>13.5738540119</v>
       </c>
-      <c r="X24">
+      <c r="X28">
         <v>13.784768872000001</v>
       </c>
-      <c r="Y24">
+      <c r="Y28">
         <v>13.8350142724</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29">
         <v>76.539524799999995</v>
       </c>
-      <c r="C25">
+      <c r="C29">
         <v>37.219631873700003</v>
       </c>
-      <c r="D25">
+      <c r="D29">
         <v>25.407926000500002</v>
       </c>
-      <c r="E25">
+      <c r="E29">
         <v>25.407926000500002</v>
       </c>
-      <c r="F25">
+      <c r="F29">
         <v>18.231084944900001</v>
       </c>
-      <c r="G25">
+      <c r="G29">
         <v>15.9022061758</v>
       </c>
-      <c r="H25">
+      <c r="H29">
         <v>14.334589317000001</v>
       </c>
-      <c r="I25">
+      <c r="I29">
         <v>13.355792874400001</v>
       </c>
-      <c r="J25">
+      <c r="J29">
         <v>13.704629744</v>
       </c>
-      <c r="K25">
+      <c r="K29">
         <v>13.5174492254</v>
       </c>
-      <c r="L25">
+      <c r="L29">
         <v>13.455847864000001</v>
       </c>
-      <c r="M25">
+      <c r="M29">
         <v>13.265079008500001</v>
       </c>
-      <c r="N25">
+      <c r="N29">
         <v>13.3117277822</v>
       </c>
-      <c r="O25">
+      <c r="O29">
         <v>13.3520829526</v>
       </c>
-      <c r="P25">
+      <c r="P29">
         <v>13.212053732699999</v>
       </c>
-      <c r="Q25">
+      <c r="Q29">
         <v>13.365067678999999</v>
       </c>
-      <c r="R25">
+      <c r="R29">
         <v>13.3115493523</v>
       </c>
-      <c r="S25">
+      <c r="S29">
         <v>13.382009050200001</v>
       </c>
-      <c r="T25">
+      <c r="T29">
         <v>13.382009050200001</v>
       </c>
-      <c r="U25">
+      <c r="U29">
         <v>13.374947645400001</v>
       </c>
-      <c r="V25">
+      <c r="V29">
         <v>13.5558736416</v>
       </c>
-      <c r="W25">
+      <c r="W29">
         <v>13.758500983099999</v>
       </c>
-      <c r="X25">
+      <c r="X29">
         <v>13.748753260200001</v>
       </c>
-      <c r="Y25">
+      <c r="Y29">
         <v>13.6965664472</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26">
-        <v>76.496251984099999</v>
-      </c>
-      <c r="C26">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30">
+        <v>73.496251984099999</v>
+      </c>
+      <c r="C30">
         <v>37.156918877899997</v>
       </c>
-      <c r="D26">
+      <c r="D30">
         <v>25.248227247100001</v>
       </c>
-      <c r="E26">
+      <c r="E30">
         <v>25.248227247100001</v>
       </c>
-      <c r="F26">
+      <c r="F30">
         <v>17.959432450600001</v>
       </c>
-      <c r="G26">
+      <c r="G30">
         <v>15.8062748129</v>
       </c>
-      <c r="H26">
+      <c r="H30">
         <v>14.3927472173</v>
       </c>
-      <c r="I26">
+      <c r="I30">
         <v>13.1986012197</v>
       </c>
-      <c r="J26">
+      <c r="J30">
         <v>13.6046347574</v>
       </c>
-      <c r="K26">
+      <c r="K30">
         <v>13.725309854300001</v>
       </c>
-      <c r="L26">
+      <c r="L30">
         <v>13.5164493071</v>
       </c>
-      <c r="M26">
+      <c r="M30">
         <v>13.3306934648</v>
       </c>
-      <c r="N26">
+      <c r="N30">
         <v>13.2568234653</v>
       </c>
-      <c r="O26">
+      <c r="O30">
         <v>13.4116528969</v>
       </c>
-      <c r="P26">
+      <c r="P30">
         <v>13.4163216824</v>
       </c>
-      <c r="Q26">
+      <c r="Q30">
         <v>13.918383693099999</v>
       </c>
-      <c r="R26">
+      <c r="R30">
         <v>13.665295414099999</v>
       </c>
-      <c r="S26">
+      <c r="S30">
         <v>13.654636593099999</v>
       </c>
-      <c r="T26">
+      <c r="T30">
         <v>13.654636593099999</v>
       </c>
-      <c r="U26">
+      <c r="U30">
         <v>13.684577691399999</v>
       </c>
-      <c r="V26">
+      <c r="V30">
         <v>13.874608352199999</v>
       </c>
-      <c r="W26">
+      <c r="W30">
         <v>13.8672303527</v>
       </c>
-      <c r="X26">
+      <c r="X30">
         <v>15.0933784724</v>
       </c>
-      <c r="Y26">
+      <c r="Y30">
         <v>14.0933275488</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27">
-        <v>76.053232523000005</v>
-      </c>
-      <c r="C27">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31">
+        <v>73.053232523000005</v>
+      </c>
+      <c r="C31">
         <v>37.260263373699999</v>
       </c>
-      <c r="D27">
+      <c r="D31">
         <v>25.1644429374</v>
       </c>
-      <c r="E27">
+      <c r="E31">
         <v>25.1644429374</v>
       </c>
-      <c r="F27">
+      <c r="F31">
         <v>17.9869177687</v>
       </c>
-      <c r="G27">
+      <c r="G31">
         <v>15.7219587661</v>
       </c>
-      <c r="H27">
+      <c r="H31">
         <v>14.3340046826</v>
       </c>
-      <c r="I27">
+      <c r="I31">
         <v>13.252832871500001</v>
       </c>
-      <c r="J27">
+      <c r="J31">
         <v>13.8685002844</v>
       </c>
-      <c r="K27">
+      <c r="K31">
         <v>13.475728592299999</v>
       </c>
-      <c r="L27">
+      <c r="L31">
         <v>13.3663466902</v>
       </c>
-      <c r="M27">
+      <c r="M31">
         <v>13.2244601408</v>
       </c>
-      <c r="N27">
+      <c r="N31">
         <v>13.234841447999999</v>
       </c>
-      <c r="O27">
+      <c r="O31">
         <v>13.2667685665</v>
       </c>
-      <c r="P27">
+      <c r="P31">
         <v>13.3736548178</v>
       </c>
-      <c r="Q27">
+      <c r="Q31">
         <v>13.232263293100001</v>
       </c>
-      <c r="R27">
+      <c r="R31">
         <v>13.272125017800001</v>
       </c>
-      <c r="S27">
+      <c r="S31">
         <v>13.255233386</v>
       </c>
-      <c r="T27">
+      <c r="T31">
         <v>13.255233386</v>
       </c>
-      <c r="U27">
+      <c r="U31">
         <v>13.332850414499999</v>
       </c>
-      <c r="V27">
+      <c r="V31">
         <v>13.4177921504</v>
       </c>
-      <c r="W27">
+      <c r="W31">
         <v>13.4683513823</v>
       </c>
-      <c r="X27">
+      <c r="X31">
         <v>13.395884347399999</v>
       </c>
-      <c r="Y27">
+      <c r="Y31">
         <v>13.423021884900001</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28">
-        <v>77.120643516300007</v>
-      </c>
-      <c r="C28">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32">
+        <v>74.120643516300007</v>
+      </c>
+      <c r="C32">
         <v>37.433510960600003</v>
       </c>
-      <c r="D28">
+      <c r="D32">
         <v>25.425069486999998</v>
       </c>
-      <c r="E28">
+      <c r="E32">
         <v>25.425069486999998</v>
       </c>
-      <c r="F28">
+      <c r="F32">
         <v>18.0550294548</v>
       </c>
-      <c r="G28">
+      <c r="G32">
         <v>15.9631257927</v>
       </c>
-      <c r="H28">
+      <c r="H32">
         <v>14.2933254171</v>
       </c>
-      <c r="I28">
+      <c r="I32">
         <v>13.2464255783</v>
       </c>
-      <c r="J28">
+      <c r="J32">
         <v>13.8235181728</v>
       </c>
-      <c r="K28">
+      <c r="K32">
         <v>13.707425015</v>
       </c>
-      <c r="L28">
+      <c r="L32">
         <v>13.5317200687</v>
       </c>
-      <c r="M28">
+      <c r="M32">
         <v>13.158424479300001</v>
       </c>
-      <c r="N28">
+      <c r="N32">
         <v>13.3124513709</v>
       </c>
-      <c r="O28">
+      <c r="O32">
         <v>13.227287387100001</v>
       </c>
-      <c r="P28">
+      <c r="P32">
         <v>13.2916078315</v>
       </c>
-      <c r="Q28">
+      <c r="Q32">
         <v>13.284988948800001</v>
       </c>
-      <c r="R28">
+      <c r="R32">
         <v>13.279594206100001</v>
       </c>
-      <c r="S28">
+      <c r="S32">
         <v>13.413831952900001</v>
       </c>
-      <c r="T28">
+      <c r="T32">
         <v>13.413831952900001</v>
       </c>
-      <c r="U28">
+      <c r="U32">
         <v>13.2911001746</v>
       </c>
-      <c r="V28">
+      <c r="V32">
         <v>13.712254466399999</v>
       </c>
-      <c r="W28">
+      <c r="W32">
         <v>13.3723260673</v>
       </c>
-      <c r="X28">
+      <c r="X32">
         <v>13.532296413199999</v>
       </c>
-      <c r="Y28">
+      <c r="Y32">
         <v>13.6807836864</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33">
         <v>75.877690611199995</v>
       </c>
-      <c r="C29">
+      <c r="C33">
         <v>38.371762355000001</v>
       </c>
-      <c r="D29">
+      <c r="D33">
         <v>27.6804789344</v>
       </c>
-      <c r="E29">
+      <c r="E33">
         <v>27.6804789344</v>
       </c>
-      <c r="F29">
+      <c r="F33">
         <v>19.280618204500001</v>
       </c>
-      <c r="G29">
+      <c r="G33">
         <v>16.732927076199999</v>
       </c>
-      <c r="H29">
+      <c r="H33">
         <v>15.2200767644</v>
       </c>
-      <c r="I29">
+      <c r="I33">
         <v>14.443932138199999</v>
       </c>
-      <c r="J29">
+      <c r="J33">
         <v>14.4406307894</v>
       </c>
-      <c r="K29">
+      <c r="K33">
         <v>14.7024380558</v>
       </c>
-      <c r="L29">
+      <c r="L33">
         <v>14.213585388</v>
       </c>
-      <c r="M29">
+      <c r="M33">
         <v>14.037379100900001</v>
       </c>
-      <c r="N29">
+      <c r="N33">
         <v>13.900294369899999</v>
       </c>
-      <c r="O29">
+      <c r="O33">
         <v>13.8510370451</v>
       </c>
-      <c r="P29">
+      <c r="P33">
         <v>13.636097642199999</v>
       </c>
-      <c r="Q29">
+      <c r="Q33">
         <v>13.858629002700001</v>
       </c>
-      <c r="R29">
+      <c r="R33">
         <v>13.771852043699999</v>
       </c>
-      <c r="S29">
+      <c r="S33">
         <v>13.538006171599999</v>
       </c>
-      <c r="T29">
+      <c r="T33">
         <v>13.538006171599999</v>
       </c>
-      <c r="U29">
+      <c r="U33">
         <v>13.9273766415</v>
       </c>
-      <c r="V29">
+      <c r="V33">
         <v>13.707770427</v>
       </c>
-      <c r="W29">
+      <c r="W33">
         <v>13.596704493600001</v>
       </c>
-      <c r="X29">
+      <c r="X33">
         <v>13.729675071999999</v>
       </c>
-      <c r="Y29">
+      <c r="Y33">
         <v>13.7965385379</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34">
         <v>74.076523947699997</v>
       </c>
-      <c r="C30">
+      <c r="C34">
         <v>37.153668847399999</v>
       </c>
-      <c r="D30">
+      <c r="D34">
         <v>25.386643097099999</v>
       </c>
-      <c r="E30">
+      <c r="E34">
         <v>25.386643097099999</v>
       </c>
-      <c r="F30">
+      <c r="F34">
         <v>17.762486050300001</v>
       </c>
-      <c r="G30">
+      <c r="G34">
         <v>15.756860375</v>
       </c>
-      <c r="H30">
+      <c r="H34">
         <v>14.2173766297</v>
       </c>
-      <c r="I30">
+      <c r="I34">
         <v>13.2648401808</v>
       </c>
-      <c r="J30">
+      <c r="J34">
         <v>13.760818993499999</v>
       </c>
-      <c r="K30">
+      <c r="K34">
         <v>13.218847097799999</v>
       </c>
-      <c r="L30">
+      <c r="L34">
         <v>13.554200268700001</v>
       </c>
-      <c r="M30">
+      <c r="M34">
         <v>13.1962674191</v>
       </c>
-      <c r="N30">
+      <c r="N34">
         <v>13.2826662014</v>
       </c>
-      <c r="O30">
+      <c r="O34">
         <v>13.3901157702</v>
       </c>
-      <c r="P30">
+      <c r="P34">
         <v>13.426512322100001</v>
       </c>
-      <c r="Q30">
+      <c r="Q34">
         <v>13.313487606800001</v>
       </c>
-      <c r="R30">
+      <c r="R34">
         <v>13.3577394188</v>
       </c>
-      <c r="S30">
+      <c r="S34">
         <v>13.4205155757</v>
       </c>
-      <c r="T30">
+      <c r="T34">
         <v>13.4205155757</v>
       </c>
-      <c r="U30">
+      <c r="U34">
         <v>13.3949408793</v>
       </c>
-      <c r="V30">
+      <c r="V34">
         <v>13.3206638857</v>
       </c>
-      <c r="W30">
+      <c r="W34">
         <v>13.590833674500001</v>
       </c>
-      <c r="X30">
+      <c r="X34">
         <v>13.5210490102</v>
       </c>
-      <c r="Y30">
+      <c r="Y34">
         <v>13.6109492829</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31">
-        <v>76.423227947800001</v>
-      </c>
-      <c r="C31">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35">
+        <v>74.423227947800001</v>
+      </c>
+      <c r="C35">
         <v>37.3291858897</v>
       </c>
-      <c r="D31">
+      <c r="D35">
         <v>25.119628991999999</v>
       </c>
-      <c r="E31">
+      <c r="E35">
         <v>25.119628991999999</v>
       </c>
-      <c r="F31">
+      <c r="F35">
         <v>17.936908432700001</v>
       </c>
-      <c r="G31">
+      <c r="G35">
         <v>15.7970726435</v>
       </c>
-      <c r="H31">
+      <c r="H35">
         <v>14.103979659</v>
       </c>
-      <c r="I31">
+      <c r="I35">
         <v>13.2703651932</v>
       </c>
-      <c r="J31">
+      <c r="J35">
         <v>13.6726884143</v>
       </c>
-      <c r="K31">
+      <c r="K35">
         <v>13.6037951103</v>
       </c>
-      <c r="L31">
+      <c r="L35">
         <v>13.3404514515</v>
       </c>
-      <c r="M31">
+      <c r="M35">
         <v>13.1832590073</v>
       </c>
-      <c r="N31">
+      <c r="N35">
         <v>13.2936341168</v>
       </c>
-      <c r="O31">
+      <c r="O35">
         <v>13.2288612814</v>
       </c>
-      <c r="P31">
+      <c r="P35">
         <v>13.3177268972</v>
       </c>
-      <c r="Q31">
+      <c r="Q35">
         <v>13.2706802089</v>
       </c>
-      <c r="R31">
+      <c r="R35">
         <v>13.357002013700001</v>
       </c>
-      <c r="S31">
+      <c r="S35">
         <v>13.490706444400001</v>
       </c>
-      <c r="T31">
+      <c r="T35">
         <v>13.490706444400001</v>
       </c>
-      <c r="U31">
+      <c r="U35">
         <v>13.3731345287</v>
       </c>
-      <c r="V31">
+      <c r="V35">
         <v>13.853575724400001</v>
       </c>
-      <c r="W31">
+      <c r="W35">
         <v>13.404206999299999</v>
       </c>
-      <c r="X31">
+      <c r="X35">
         <v>13.6873721729</v>
       </c>
-      <c r="Y31">
+      <c r="Y35">
         <v>13.795685863799999</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36">
         <v>76.618395575299999</v>
       </c>
-      <c r="C32">
+      <c r="C36">
         <v>37.193249900200001</v>
       </c>
-      <c r="D32">
+      <c r="D36">
         <v>25.168326552100002</v>
       </c>
-      <c r="E32">
+      <c r="E36">
         <v>25.168326552100002</v>
       </c>
-      <c r="F32">
+      <c r="F36">
         <v>17.937697156199999</v>
       </c>
-      <c r="G32">
+      <c r="G36">
         <v>15.728541726</v>
       </c>
-      <c r="H32">
+      <c r="H36">
         <v>14.1301812288</v>
       </c>
-      <c r="I32">
+      <c r="I36">
         <v>13.242262476000001</v>
       </c>
-      <c r="J32">
+      <c r="J36">
         <v>13.573752559500001</v>
       </c>
-      <c r="K32">
+      <c r="K36">
         <v>13.623086861799999</v>
       </c>
-      <c r="L32">
+      <c r="L36">
         <v>13.3504364231</v>
       </c>
-      <c r="M32">
+      <c r="M36">
         <v>13.434208890200001</v>
       </c>
-      <c r="N32">
+      <c r="N36">
         <v>13.255709857099999</v>
       </c>
-      <c r="O32">
+      <c r="O36">
         <v>13.175820610000001</v>
       </c>
-      <c r="P32">
+      <c r="P36">
         <v>13.3119070017</v>
       </c>
-      <c r="Q32">
+      <c r="Q36">
         <v>13.286641794399999</v>
       </c>
-      <c r="R32">
+      <c r="R36">
         <v>13.327769898</v>
       </c>
-      <c r="S32">
+      <c r="S36">
         <v>13.359563983499999</v>
       </c>
-      <c r="T32">
+      <c r="T36">
         <v>13.359563983499999</v>
       </c>
-      <c r="U32">
+      <c r="U36">
         <v>13.302871419500001</v>
       </c>
-      <c r="V32">
+      <c r="V36">
         <v>13.459801350599999</v>
       </c>
-      <c r="W32">
+      <c r="W36">
         <v>13.6114691772</v>
       </c>
-      <c r="X32">
+      <c r="X36">
         <v>13.368102567199999</v>
       </c>
-      <c r="Y32">
+      <c r="Y36">
         <v>13.6822569178</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37">
         <v>75.279577231499999</v>
       </c>
-      <c r="C33">
+      <c r="C37">
         <v>37.629607844900001</v>
       </c>
-      <c r="D33">
+      <c r="D37">
         <v>26.3804651574</v>
       </c>
-      <c r="E33">
+      <c r="E37">
         <v>26.3804651574</v>
       </c>
-      <c r="F33">
+      <c r="F37">
         <v>18.623855058</v>
       </c>
-      <c r="G33">
+      <c r="G37">
         <v>16.397916553999998</v>
       </c>
-      <c r="H33">
+      <c r="H37">
         <v>15.0494187802</v>
       </c>
-      <c r="I33">
+      <c r="I37">
         <v>14.1267235563</v>
       </c>
-      <c r="J33">
+      <c r="J37">
         <v>13.6946609574</v>
       </c>
-      <c r="K33">
+      <c r="K37">
         <v>13.614253789799999</v>
       </c>
-      <c r="L33">
+      <c r="L37">
         <v>13.4559674752</v>
       </c>
-      <c r="M33">
+      <c r="M37">
         <v>13.1543951994</v>
       </c>
-      <c r="N33">
+      <c r="N37">
         <v>13.2528190551</v>
       </c>
-      <c r="O33">
+      <c r="O37">
         <v>13.3029523446</v>
       </c>
-      <c r="P33">
+      <c r="P37">
         <v>13.335741216600001</v>
       </c>
-      <c r="Q33">
+      <c r="Q37">
         <v>13.336051100400001</v>
       </c>
-      <c r="R33">
+      <c r="R37">
         <v>13.2706055999</v>
       </c>
-      <c r="S33">
+      <c r="S37">
         <v>13.516083762599999</v>
       </c>
-      <c r="T33">
+      <c r="T37">
         <v>13.516083762599999</v>
       </c>
-      <c r="U33">
+      <c r="U37">
         <v>13.4402901145</v>
       </c>
-      <c r="V33">
+      <c r="V37">
         <v>13.6070814584</v>
       </c>
-      <c r="W33">
+      <c r="W37">
         <v>13.4973055893</v>
       </c>
-      <c r="X33">
+      <c r="X37">
         <v>13.7000004342</v>
       </c>
-      <c r="Y33">
+      <c r="Y37">
         <v>13.609971076200001</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
-      <c r="B34" s="3">
-        <f>AVERAGE(B24:B33)</f>
-        <v>76.108462632539997</v>
-      </c>
-      <c r="C34" s="3">
-        <f t="shared" ref="C34:Y34" si="2">AVERAGE(C24:C33)</f>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="3">
+        <f>AVERAGE(B28:B37)</f>
+        <v>74.608462632539997</v>
+      </c>
+      <c r="C38" s="3">
+        <f t="shared" ref="C38:Y38" si="6">AVERAGE(C28:C37)</f>
         <v>37.399145115250001</v>
       </c>
-      <c r="D34" s="3">
-        <f t="shared" si="2"/>
+      <c r="D38" s="3">
+        <f t="shared" si="6"/>
         <v>25.616824681130005</v>
       </c>
-      <c r="E34" s="3">
-        <f t="shared" si="2"/>
+      <c r="E38" s="3">
+        <f t="shared" si="6"/>
         <v>25.616824681130005</v>
       </c>
-      <c r="F34" s="3">
-        <f t="shared" si="2"/>
+      <c r="F38" s="3">
+        <f t="shared" si="6"/>
         <v>18.192384949199997</v>
       </c>
-      <c r="G34" s="3">
-        <f t="shared" si="2"/>
+      <c r="G38" s="3">
+        <f t="shared" si="6"/>
         <v>15.99103559243</v>
       </c>
-      <c r="H34" s="3">
-        <f t="shared" si="2"/>
+      <c r="H38" s="3">
+        <f t="shared" si="6"/>
         <v>14.4267221747</v>
       </c>
-      <c r="I34" s="3">
-        <f t="shared" si="2"/>
+      <c r="I38" s="3">
+        <f t="shared" si="6"/>
         <v>13.463165347310001</v>
       </c>
-      <c r="J34" s="3">
-        <f t="shared" si="2"/>
+      <c r="J38" s="3">
+        <f t="shared" si="6"/>
         <v>13.813584953769999</v>
       </c>
-      <c r="K34" s="3">
-        <f t="shared" si="2"/>
+      <c r="K38" s="3">
+        <f t="shared" si="6"/>
         <v>13.686709889880001</v>
       </c>
-      <c r="L34" s="3">
-        <f t="shared" si="2"/>
+      <c r="L38" s="3">
+        <f t="shared" si="6"/>
         <v>13.522350167209998</v>
       </c>
-      <c r="M34" s="3">
-        <f t="shared" si="2"/>
+      <c r="M38" s="3">
+        <f t="shared" si="6"/>
         <v>13.319988102029999</v>
       </c>
-      <c r="N34" s="3">
-        <f t="shared" si="2"/>
+      <c r="N38" s="3">
+        <f t="shared" si="6"/>
         <v>13.353381662059999</v>
       </c>
-      <c r="O34" s="3">
-        <f t="shared" si="2"/>
+      <c r="O38" s="3">
+        <f t="shared" si="6"/>
         <v>13.355361129189998</v>
       </c>
-      <c r="P34" s="3">
-        <f t="shared" si="2"/>
+      <c r="P38" s="3">
+        <f t="shared" si="6"/>
         <v>13.364253414750001</v>
       </c>
-      <c r="Q34" s="3">
-        <f t="shared" si="2"/>
+      <c r="Q38" s="3">
+        <f t="shared" si="6"/>
         <v>13.415471613639999</v>
       </c>
-      <c r="R34" s="3">
-        <f t="shared" si="2"/>
+      <c r="R38" s="3">
+        <f t="shared" si="6"/>
         <v>13.404770356319997</v>
       </c>
-      <c r="S34" s="3">
-        <f t="shared" si="2"/>
+      <c r="S38" s="3">
+        <f t="shared" si="6"/>
         <v>13.434462165939999</v>
       </c>
-      <c r="T34" s="3">
-        <f t="shared" si="2"/>
+      <c r="T38" s="3">
+        <f t="shared" si="6"/>
         <v>13.434462165939999</v>
       </c>
-      <c r="U34" s="3">
-        <f t="shared" si="2"/>
+      <c r="U38" s="3">
+        <f t="shared" si="6"/>
         <v>13.44827986816</v>
       </c>
-      <c r="V34" s="3">
-        <f t="shared" si="2"/>
+      <c r="V38" s="3">
+        <f t="shared" si="6"/>
         <v>13.588837351230001</v>
       </c>
-      <c r="W34" s="3">
-        <f t="shared" si="2"/>
+      <c r="W38" s="3">
+        <f t="shared" si="6"/>
         <v>13.57407827312</v>
       </c>
-      <c r="X34" s="3">
-        <f t="shared" si="2"/>
+      <c r="X38" s="3">
+        <f t="shared" si="6"/>
         <v>13.756128062170001</v>
       </c>
-      <c r="Y34" s="3">
-        <f t="shared" si="2"/>
+      <c r="Y38" s="3">
+        <f t="shared" si="6"/>
         <v>13.722411551830001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="2">
+        <f>$B$38/B38</f>
+        <v>1</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" ref="C39:Y39" si="7">$B$38/C38</f>
+        <v>1.994924279756261</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="7"/>
+        <v>2.9124789493327978</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="7"/>
+        <v>2.9124789493327978</v>
+      </c>
+      <c r="F39" s="2">
+        <f t="shared" si="7"/>
+        <v>4.1010820099110132</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="7"/>
+        <v>4.665642959850512</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.1715463657697738</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.5416732029846969</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.4010934078468802</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.4511612529835052</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.5174183266941386</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.6012409366318794</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.5872335952562224</v>
+      </c>
+      <c r="O39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.5864054824749614</v>
+      </c>
+      <c r="P39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.5826884089308972</v>
+      </c>
+      <c r="Q39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.5613745667116801</v>
+      </c>
+      <c r="R39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.5658143070958372</v>
+      </c>
+      <c r="S39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.5535131746243369</v>
+      </c>
+      <c r="T39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.5535131746243369</v>
+      </c>
+      <c r="U39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.5478071072258226</v>
+      </c>
+      <c r="V39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.4904228157375634</v>
+      </c>
+      <c r="W39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.4963925455095559</v>
+      </c>
+      <c r="X39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.4236528109764244</v>
+      </c>
+      <c r="Y39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.4369789414011791</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="2">
+        <f>B39/B1</f>
+        <v>1</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" ref="C40:Y40" si="8">C39/C1</f>
+        <v>0.99746213987813048</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.97082631644426598</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.72811973733319946</v>
+      </c>
+      <c r="F40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.82021640198220269</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.77760715997508534</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.73879233796711052</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.69270915037308711</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.60012148976076451</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.54511612529835052</v>
+      </c>
+      <c r="L40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.50158348424492172</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.46677007805265663</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.42978719963509404</v>
+      </c>
+      <c r="O40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.39902896303392582</v>
+      </c>
+      <c r="P40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.37217922726205982</v>
+      </c>
+      <c r="Q40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.34758591041948</v>
+      </c>
+      <c r="R40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.32740084159387278</v>
+      </c>
+      <c r="S40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.30852850970135204</v>
+      </c>
+      <c r="T40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.29229016708549144</v>
+      </c>
+      <c r="U40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.27739035536129114</v>
+      </c>
+      <c r="V40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.26144870551131255</v>
+      </c>
+      <c r="W40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.2498360247958889</v>
+      </c>
+      <c r="X40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.23581099178158366</v>
+      </c>
+      <c r="Y40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.22654078922504914</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="A28:A38"/>
     <mergeCell ref="A2:A12"/>
-    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="A15:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>